<commit_message>
Correção bug: coluna só exite na base A e coluna só exite base B
</commit_message>
<xml_diff>
--- a/Arquivos/Saida.xlsx
+++ b/Arquivos/Saida.xlsx
@@ -449,14 +449,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -492,6 +490,9 @@
       <c r="D2">
         <v>10</v>
       </c>
+      <c r="F2">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -506,6 +507,9 @@
       <c r="D3">
         <v>20</v>
       </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -520,6 +524,9 @@
       <c r="D4">
         <v>30</v>
       </c>
+      <c r="F4">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -534,6 +541,9 @@
       <c r="D5">
         <v>40</v>
       </c>
+      <c r="F5">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -548,6 +558,9 @@
       <c r="D6">
         <v>50</v>
       </c>
+      <c r="F6">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
@@ -562,6 +575,9 @@
       <c r="D7">
         <v>60</v>
       </c>
+      <c r="F7">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -576,6 +592,9 @@
       <c r="D8">
         <v>70</v>
       </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -590,6 +609,9 @@
       <c r="D9">
         <v>80</v>
       </c>
+      <c r="F9">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -604,6 +626,9 @@
       <c r="D10">
         <v>90</v>
       </c>
+      <c r="F10">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -618,6 +643,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -632,6 +660,9 @@
       <c r="D12">
         <v>11</v>
       </c>
+      <c r="F12">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -646,6 +677,9 @@
       <c r="D13">
         <v>21</v>
       </c>
+      <c r="F13">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -660,6 +694,9 @@
       <c r="D14">
         <v>31</v>
       </c>
+      <c r="F14">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -674,6 +711,9 @@
       <c r="D15">
         <v>41</v>
       </c>
+      <c r="F15">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
@@ -687,6 +727,9 @@
       </c>
       <c r="D16">
         <v>51</v>
+      </c>
+      <c r="F16">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>